<commit_message>
edti: todo report, backup sqm 20191221
</commit_message>
<xml_diff>
--- a/To-do list.xlsx
+++ b/To-do list.xlsx
@@ -15,14 +15,14 @@
     <sheet name="To do" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$3:$C$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$3:$C$40</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t xml:space="preserve">
  To Do</t>
@@ -197,25 +197,76 @@
     <t>Demo web react-app</t>
   </si>
   <si>
-    <t>Bổ sung báo cáo hoàn thiện các diagram</t>
-  </si>
-  <si>
-    <t>Hoàn thiện các chức năng</t>
-  </si>
-  <si>
-    <t>Thêm trải nghiệm người dùng</t>
-  </si>
-  <si>
-    <t>Deploy and hosting with docker</t>
-  </si>
-  <si>
-    <t>review</t>
-  </si>
-  <si>
-    <t>Báo cáo Tiểu luận chuyên ngành</t>
-  </si>
-  <si>
-    <t>Admin UI, Load data with API(page tour, detail tour, index, admin tours</t>
+    <t>Routing page</t>
+  </si>
+  <si>
+    <t>https://github.com/ithoangtan/KinhDoanhTourDuLich</t>
+  </si>
+  <si>
+    <t>Sort, search</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa giao diện chính</t>
+  </si>
+  <si>
+    <t>Test và chỉnh sửa chức năng chính</t>
+  </si>
+  <si>
+    <t>Làm báo cáo</t>
+  </si>
+  <si>
+    <t>báo cáo sơ đồ</t>
+  </si>
+  <si>
+    <t>miêu tả sơ đồ</t>
+  </si>
+  <si>
+    <t>Hoàn thành báo cáo nộp lần 1</t>
+  </si>
+  <si>
+    <t>Nộp báo cáo xin ý kiến lần 1</t>
+  </si>
+  <si>
+    <t>Thanh toán online</t>
+  </si>
+  <si>
+    <t>đã có demo</t>
+  </si>
+  <si>
+    <t>khai báo với ngân lượng, onepay</t>
+  </si>
+  <si>
+    <t>In lịch trình tour</t>
+  </si>
+  <si>
+    <t>print-js</t>
+  </si>
+  <si>
+    <t>Sử dụng để in(trạng thái gọi API của clinent</t>
+  </si>
+  <si>
+    <t>Chỉnh báo cáo theo yêu cầu của thầy nếu có</t>
+  </si>
+  <si>
+    <t>Chức năng report admin(dashroad)</t>
+  </si>
+  <si>
+    <t>Thêm cơ sở dữ liệu mẫu</t>
+  </si>
+  <si>
+    <t>mySQL</t>
+  </si>
+  <si>
+    <t>Tinh chỉnh báo cáo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deadline nộp báo cáo cuối cùng </t>
+  </si>
+  <si>
+    <t>Xin chữ ký của thầy Vinh</t>
+  </si>
+  <si>
+    <t>Báo cáo Tiểu luận theo kế hoạch</t>
   </si>
 </sst>
 </file>
@@ -225,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -291,6 +342,16 @@
       <sz val="14"/>
       <color rgb="FF434343"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -399,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -464,6 +525,8 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -475,7 +538,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -767,11 +842,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -783,13 +858,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="52.5" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26"/>
       <c r="C1" s="1" t="str">
-        <f>CONCATENATE(COUNTIF($A$4:$A$51,TRUE), "/", COUNTA($C$4:$C$51), " completed  ")</f>
-        <v xml:space="preserve">12/23 completed  </v>
+        <f>CONCATENATE(COUNTIF($A$4:$A$40,TRUE), "/", COUNTA($C$4:$C$40), " completed  ")</f>
+        <v xml:space="preserve">17/33 completed  </v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1041,9 +1116,9 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="26.25" customHeight="1">
       <c r="A16" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" s="20">
         <v>43783</v>
@@ -1054,14 +1129,12 @@
       <c r="D16" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>54</v>
-      </c>
+      <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="26.25" customHeight="1">
       <c r="A17" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" s="20">
         <v>43784</v>
@@ -1077,7 +1150,7 @@
     </row>
     <row r="18" spans="1:6" ht="26.25" customHeight="1">
       <c r="A18" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="20">
         <v>43785</v>
@@ -1093,7 +1166,7 @@
     </row>
     <row r="19" spans="1:6" ht="26.25" customHeight="1">
       <c r="A19" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="20">
         <v>43786</v>
@@ -1111,7 +1184,7 @@
     </row>
     <row r="20" spans="1:6" ht="26.25" customHeight="1">
       <c r="A20" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="21">
         <v>43787</v>
@@ -1127,13 +1200,15 @@
       <c r="A21" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B21" s="20">
-        <v>43788</v>
+      <c r="B21" s="21">
+        <v>43812</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
     </row>
@@ -1141,184 +1216,236 @@
       <c r="A22" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B22" s="20">
-        <v>43789</v>
+      <c r="B22" s="21">
+        <v>43813</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="26.25" customHeight="1">
       <c r="A23" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B23" s="20">
-        <v>43790</v>
+      <c r="B23" s="21">
+        <v>43818</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="14"/>
+        <v>51</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="F23" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1">
       <c r="A24" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="20">
-        <v>43791</v>
-      </c>
-      <c r="C24" s="13"/>
+      <c r="B24" s="21">
+        <v>43819</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="F24" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="26.25" customHeight="1">
       <c r="A25" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="20">
-        <v>43792</v>
+      <c r="B25" s="21">
+        <v>43820</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+        <v>53</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="26.25" customHeight="1">
       <c r="A26" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="20">
-        <v>43793</v>
+      <c r="B26" s="21">
+        <v>43821</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="26.25" customHeight="1">
       <c r="A27" s="9" t="b">
         <v>0</v>
       </c>
       <c r="B27" s="21">
-        <v>43794</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>53</v>
+        <v>43822</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" ht="26.25" customHeight="1">
       <c r="A28" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="20">
-        <v>43795</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="B28" s="21">
+        <v>43823</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="26.25" customHeight="1">
       <c r="A29" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="20">
-        <v>43796</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="B29" s="21">
+        <v>43824</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="26.25" customHeight="1">
       <c r="A30" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="20">
-        <v>43797</v>
-      </c>
-      <c r="C30" s="13"/>
+      <c r="B30" s="21">
+        <v>43825</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" ht="26.25" customHeight="1">
       <c r="A31" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="20">
-        <v>43798</v>
-      </c>
-      <c r="C31" s="13"/>
+      <c r="B31" s="21">
+        <v>43826</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="F31" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="26.25" customHeight="1">
       <c r="A32" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="20">
-        <v>43799</v>
-      </c>
-      <c r="C32" s="13"/>
+      <c r="B32" s="21">
+        <v>43827</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
+      <c r="F32" s="23" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="26.25" customHeight="1">
       <c r="A33" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="20">
-        <v>43800</v>
-      </c>
-      <c r="C33" s="13"/>
+      <c r="B33" s="21">
+        <v>43828</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" ht="26.25" customHeight="1">
       <c r="A34" s="9" t="b">
         <v>0</v>
       </c>
       <c r="B34" s="21">
-        <v>43801</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
+        <v>43829</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" ht="26.25" customHeight="1">
       <c r="A35" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="13"/>
+      <c r="B35" s="21">
+        <v>43833</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" ht="26.25" customHeight="1">
       <c r="A36" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="21">
+        <v>43834</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -1327,7 +1454,9 @@
       <c r="A37" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21">
+        <v>43835</v>
+      </c>
       <c r="C37" s="13"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
@@ -1337,7 +1466,9 @@
       <c r="A38" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="20"/>
+      <c r="B38" s="21">
+        <v>43836</v>
+      </c>
       <c r="C38" s="13"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1347,142 +1478,49 @@
       <c r="A39" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="20"/>
+      <c r="B39" s="21">
+        <v>43837</v>
+      </c>
       <c r="C39" s="13"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A40" s="9" t="b">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:6" ht="22.5" hidden="1" customHeight="1">
+      <c r="A40" s="9"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A41" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-    </row>
-    <row r="42" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A42" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A43" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-    </row>
-    <row r="44" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A44" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A45" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B45" s="20"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-    </row>
-    <row r="46" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A46" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A47" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-    </row>
-    <row r="48" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A48" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A49" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-    </row>
-    <row r="50" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A50" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="1:6" ht="22.5" hidden="1" customHeight="1">
-      <c r="A51" s="9"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C51"/>
+  <autoFilter ref="A3:C40"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:F51">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="B21:B39">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$A21=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A40 B4:B20 C4:F40 B23:B40">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A4=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="D21" r:id="rId2"/>
+    <hyperlink ref="D22" r:id="rId3"/>
+    <hyperlink ref="F22" r:id="rId4"/>
+    <hyperlink ref="D23" r:id="rId5"/>
+    <hyperlink ref="F23" r:id="rId6"/>
+    <hyperlink ref="F24" r:id="rId7"/>
+    <hyperlink ref="F25" r:id="rId8"/>
+    <hyperlink ref="F28" r:id="rId9"/>
+    <hyperlink ref="F29" r:id="rId10"/>
+    <hyperlink ref="F31" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
report phan mo dau va chuong 1 OK
</commit_message>
<xml_diff>
--- a/To-do list.xlsx
+++ b/To-do list.xlsx
@@ -845,8 +845,8 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -864,7 +864,7 @@
       <c r="B1" s="26"/>
       <c r="C1" s="1" t="str">
         <f>CONCATENATE(COUNTIF($A$4:$A$40,TRUE), "/", COUNTA($C$4:$C$40), " completed  ")</f>
-        <v xml:space="preserve">17/33 completed  </v>
+        <v xml:space="preserve">25/33 completed  </v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="21" spans="1:6" ht="26.25" customHeight="1">
       <c r="A21" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="21">
         <v>43812</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="22" spans="1:6" ht="26.25" customHeight="1">
       <c r="A22" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" s="21">
         <v>43813</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="23" spans="1:6" ht="26.25" customHeight="1">
       <c r="A23" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" s="21">
         <v>43818</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1">
       <c r="A24" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" s="21">
         <v>43819</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="25" spans="1:6" ht="26.25" customHeight="1">
       <c r="A25" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" s="21">
         <v>43820</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="26" spans="1:6" ht="26.25" customHeight="1">
       <c r="A26" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" s="21">
         <v>43821</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="27" spans="1:6" ht="26.25" customHeight="1">
       <c r="A27" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27" s="21">
         <v>43822</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="28" spans="1:6" ht="26.25" customHeight="1">
       <c r="A28" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" s="21">
         <v>43823</v>

</xml_diff>